<commit_message>
moved flight examples to separate folder
</commit_message>
<xml_diff>
--- a/examples/Imputation/Imputed_data_Example_loaded.xlsx
+++ b/examples/Imputation/Imputed_data_Example_loaded.xlsx
@@ -507,13 +507,13 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>0.940134</v>
+        <v>0.96572</v>
       </c>
       <c r="C2" t="n">
-        <v>-0.003316</v>
+        <v>-0.007924</v>
       </c>
       <c r="D2" t="n">
-        <v>0.041116</v>
+        <v>0.016931</v>
       </c>
       <c r="E2" t="n">
         <v>1</v>

</xml_diff>